<commit_message>
[Fix] B-10 not Issue
</commit_message>
<xml_diff>
--- a/F.篩選商品比較分析（驗證集經篩選）（TOP-15）.xlsx
+++ b/F.篩選商品比較分析（驗證集經篩選）（TOP-15）.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20359"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20361"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\OneDrive\碩士論文\05.Raw Data\篩選商品\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61A7E0DA-A672-4940-AC5C-2AF37E388983}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B2E2144-F18C-4AAD-9A7A-96B6DC320025}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" xr2:uid="{0CCEACF3-BF96-4B3C-80DF-3F35E77D77AE}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" firstSheet="8" activeTab="25" xr2:uid="{0CCEACF3-BF96-4B3C-80DF-3F35E77D77AE}"/>
   </bookViews>
   <sheets>
     <sheet name="A-01" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4157" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4156" uniqueCount="152">
   <si>
     <t>M-20</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1041,7 +1041,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48C5E13F-4D93-44DA-BA33-FC3BAF66818E}">
   <dimension ref="A1:AA22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:M1"/>
     </sheetView>
   </sheetViews>
@@ -18150,8 +18150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36CC5410-173A-49B5-BD31-CF8242AF6D1F}">
   <dimension ref="A1:AA22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:M1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R16" sqref="R16:S16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -19188,12 +19188,6 @@
       </c>
       <c r="Q16" s="1">
         <v>4</v>
-      </c>
-      <c r="R16" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="S16" s="1">
-        <v>3</v>
       </c>
       <c r="T16" s="1" t="s">
         <v>143</v>

</xml_diff>